<commit_message>
Modulo de edicao de dados adicionado a contas de casa e ajustando para anotacao contas
</commit_message>
<xml_diff>
--- a/controleFinanceiro.xlsx
+++ b/controleFinanceiro.xlsx
@@ -1,99 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Anotacao Contas" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contas de Casa" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Mes</t>
-  </si>
-  <si>
-    <t>Ano</t>
-  </si>
-  <si>
-    <t>Categoria Conta</t>
-  </si>
-  <si>
-    <t>Descricao</t>
-  </si>
-  <si>
-    <t>Valor</t>
-  </si>
-  <si>
-    <t>Data Compra</t>
-  </si>
-  <si>
-    <t>Pago</t>
-  </si>
-  <si>
-    <t>Observacao</t>
-  </si>
-  <si>
-    <t>Categoria</t>
-  </si>
-  <si>
-    <t>626f26e5-9189-450b-a3fd-fac383e7b720</t>
-  </si>
-  <si>
-    <t>Janeiro</t>
-  </si>
-  <si>
-    <t>Alimentação</t>
-  </si>
-  <si>
-    <t>teste</t>
-  </si>
-  <si>
-    <t>01/01/2024</t>
-  </si>
-  <si>
-    <t>Sim</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="DD/MM/YYYY"/>
+  </numFmts>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -101,36 +44,86 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -418,75 +411,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nome Contas</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Data Vencimento</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Data Pagamento</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Observacao</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>2024</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>fffae122-7220-4ec6-8929-d052b0b735f6</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>teste3</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>123</v>
       </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>10/01/2024</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modulo de edicao de dados adicionado a faculdade, falta arrumar o salvarDadosEditados que nao esta salvando os dados de forma correta
</commit_message>
<xml_diff>
--- a/controleFinanceiro.xlsx
+++ b/controleFinanceiro.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contas de Casa" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Anotacao Contas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Faculdade" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,6 +502,43 @@
       <c r="F2" t="inlineStr">
         <is>
           <t>Não</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>3e8f8227-8adf-4920-b55d-7a004e81ad98</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>02/01/2024</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>b</t>
         </is>
       </c>
     </row>
@@ -515,7 +553,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -664,12 +702,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Janeiro</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>2024</v>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>Alimentação</t>
@@ -680,8 +720,10 @@
           <t>teste2</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>125</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>521</t>
+        </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -699,47 +741,234 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>77c86141-f539-45b5-ac82-c0550867a14a</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Janeiro</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2022</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Alimentação</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>teste5</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>231</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>02/01/2024</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Nome da Materia</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Nota Atividade 1</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Nota Atividade 2</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Nota Atividade 3</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Nota Atividade 4</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Nota Mapa</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Nota SGC</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Valor Mensalidade</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Data Mensalidade</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 11</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 12</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 13</t>
+        </is>
+      </c>
+      <c r="O1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 14</t>
+        </is>
+      </c>
+      <c r="P1" s="2" t="inlineStr">
+        <is>
+          <t>Nome Matéria</t>
+        </is>
+      </c>
+      <c r="Q1" s="2" t="inlineStr">
+        <is>
+          <t>Nota MAPA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>7ad0e37b-302c-455f-aa93-eaf7d8228f33</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Engenharia de Software LL</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>127</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="L2" t="n">
+        <v/>
+      </c>
+      <c r="M2" t="n">
+        <v/>
+      </c>
+      <c r="N2" t="n">
+        <v/>
+      </c>
+      <c r="O2" t="n">
+        <v/>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Engenharia de Software xx</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>5667db64-9a3e-4d25-a4dd-df433cea8627</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Engenharia de Software</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>127</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v/>
+      </c>
+      <c r="M3" t="n">
+        <v/>
+      </c>
+      <c r="N3" t="n">
+        <v/>
+      </c>
+      <c r="O3" t="n">
+        <v/>
+      </c>
+      <c r="P3" t="n">
+        <v/>
+      </c>
+      <c r="Q3" t="n">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modulo InvestimentosSalario ajustado para manipulacao e edicao de dados, funcionando corretamente
</commit_message>
<xml_diff>
--- a/controleFinanceiro.xlsx
+++ b/controleFinanceiro.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contas de Casa" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Anotacao Contas" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Faculdade" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Investimento e Salario" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,12 +31,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -81,7 +76,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -92,23 +87,11 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
@@ -117,14 +100,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -206,10 +187,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -247,71 +228,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -339,7 +320,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -362,11 +343,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -375,13 +356,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -391,7 +372,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -400,7 +381,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -409,7 +390,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -417,10 +398,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -496,115 +477,110 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="11" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="7" max="7"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="1" max="2"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="4" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="9" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Nome Contas</t>
         </is>
       </c>
-      <c r="C1" s="13" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>Valor</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Data Vencimento</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Data Pagamento</t>
         </is>
       </c>
-      <c r="F1" s="9" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Pago</t>
         </is>
       </c>
-      <c r="G1" s="9" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Observacao</t>
         </is>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="9" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>fffae122-7220-4ec6-8929-d052b0b735f6</t>
         </is>
       </c>
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>teste3</t>
         </is>
       </c>
-      <c r="C2" s="12" t="n">
+      <c r="C2" s="5" t="n">
         <v>123</v>
       </c>
-      <c r="D2" s="9" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>10/01/2024</t>
         </is>
       </c>
-      <c r="E2" s="9" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>01/01/2024</t>
         </is>
       </c>
-      <c r="F2" s="9" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G2" s="9" t="n"/>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="9" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>3e8f8227-8adf-4920-b55d-7a004e81ad98</t>
         </is>
       </c>
-      <c r="B3" s="9" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>teste</t>
         </is>
       </c>
-      <c r="C3" s="12" t="n">
+      <c r="C3" s="5" t="n">
         <v>111</v>
       </c>
-      <c r="D3" s="9" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>02/01/2024</t>
         </is>
       </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>01/01/2024</t>
         </is>
       </c>
-      <c r="F3" s="9" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="G3" s="9" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -627,17 +603,13 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="14" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="11" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="7" max="7"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="8" max="8"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="9" max="9"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="1" max="2"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="4" max="5"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="7" max="9"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -688,131 +660,131 @@
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="9" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>ecbd5140-678a-4638-90e0-a4ee4688c365</t>
         </is>
       </c>
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>Janeiro</t>
         </is>
       </c>
-      <c r="C2" s="12" t="n">
+      <c r="C2" s="5" t="n">
         <v>2024</v>
       </c>
-      <c r="D2" s="9" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Alimentação</t>
         </is>
       </c>
-      <c r="E2" s="9" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>teste</t>
         </is>
       </c>
-      <c r="F2" s="12" t="n">
+      <c r="F2" s="5" t="n">
         <v>123</v>
       </c>
-      <c r="G2" s="9" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>01/01/2024</t>
         </is>
       </c>
-      <c r="H2" s="9" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="I2" s="9" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="9" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>7c42d6f6-6a71-40e3-aadd-65785ee56575</t>
         </is>
       </c>
-      <c r="B3" s="9" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Janeiro</t>
         </is>
       </c>
-      <c r="C3" s="12" t="n">
+      <c r="C3" s="5" t="n">
         <v>2024</v>
       </c>
-      <c r="D3" s="9" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Alimentação</t>
         </is>
       </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>teste2</t>
         </is>
       </c>
-      <c r="F3" s="12" t="n">
+      <c r="F3" s="5" t="n">
         <v>123</v>
       </c>
-      <c r="G3" s="9" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>02/01/2024</t>
         </is>
       </c>
-      <c r="H3" s="9" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="I3" s="9" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="9" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>3acecfb7-97ff-4ab4-92b2-3e9196252d93</t>
         </is>
       </c>
-      <c r="B4" s="9" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>2024</t>
         </is>
       </c>
-      <c r="C4" s="13" t="inlineStr">
+      <c r="C4" s="8" t="inlineStr">
         <is>
           <t>Janeiro</t>
         </is>
       </c>
-      <c r="D4" s="9" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Alimentação</t>
         </is>
       </c>
-      <c r="E4" s="9" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>teste2</t>
         </is>
       </c>
-      <c r="F4" s="12" t="n">
+      <c r="F4" s="5" t="n">
         <v>521</v>
       </c>
-      <c r="G4" s="9" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>02/01/2024</t>
         </is>
       </c>
-      <c r="H4" s="9" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="I4" s="9" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -835,19 +807,13 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="1" max="1"/>
-    <col width="29.29071428571428" bestFit="1" customWidth="1" style="9" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="7" max="7"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="11" min="8" max="8"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="11" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="10" max="10"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="29.33203125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" style="6" min="3" max="7"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" style="7" min="8" max="9"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="10" max="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -918,25 +884,25 @@
           <t>Engenharia de Software ll</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" s="4" t="n">
         <v>0.4</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" s="4" t="n">
         <v>3.5</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" s="5" t="n">
         <v>217</v>
       </c>
       <c r="J2" t="inlineStr">
@@ -961,25 +927,25 @@
           <t>Engenharia de software</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" s="4" t="n">
         <v>0.4</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" s="4" t="n">
         <v>3.2</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" s="5" t="n">
         <v>350</v>
       </c>
       <c r="J3" t="inlineStr">
@@ -1004,25 +970,25 @@
           <t>Engenharia de software</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="4" t="n">
         <v>0.2</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" s="4" t="n">
         <v>0.4</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" s="4" t="n">
         <v>2.5</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" s="5" t="n">
         <v>350</v>
       </c>
       <c r="J4" t="inlineStr">
@@ -1047,25 +1013,25 @@
           <t>Engenharia de software</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5" s="4" t="n">
         <v>0.4</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" s="4" t="n">
         <v>3.2</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5" s="5" t="n">
         <v>580</v>
       </c>
       <c r="J5" t="inlineStr">
@@ -1090,25 +1056,25 @@
           <t>Engenharia de software</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" s="4" t="n">
         <v>0.4</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="4" t="n">
         <v>3.2</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" s="5" t="n">
         <v>580</v>
       </c>
       <c r="J6" t="inlineStr">
@@ -1125,4 +1091,100 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mes</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Ano</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Tipo Investimento</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>c86e1f1e-aaec-470a-915f-874ae7016864</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Outubro</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2024</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Investimento</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>3811e0d5-9d25-43f8-91b2-9339859af7fa</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Maio</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Investimento</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>